<commit_message>
fitur cetak pdf aset inventaris done
</commit_message>
<xml_diff>
--- a/public/templates/template_aset_inventaris_ruangan.xlsx
+++ b/public/templates/template_aset_inventaris_ruangan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daffa Budi Prasetya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\bismillah_sip_aset\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D52F052-A1DA-4F32-80B0-83E70DA655AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12B1601-7F77-495E-A022-12D443F4ACD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{EA767793-6A0C-4171-AE55-10E9968E0A80}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
         <v>2017</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J2">
         <v>10000000</v>

</xml_diff>